<commit_message>
第十次提交： 1、用例层编写实战 login_test quit_test 模块 2、自定义unittest.TestCase SeleniumBaseCase模块
</commit_message>
<xml_diff>
--- a/element_info_datas/element_infos.xlsx
+++ b/element_info_datas/element_infos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9140"/>
+    <workbookView windowWidth="25600" windowHeight="9140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
   <si>
     <t>元素变量名</t>
   </si>
@@ -75,30 +75,18 @@
     <t>B</t>
   </si>
   <si>
-    <t>bug_link</t>
-  </si>
-  <si>
-    <t>bug链接[%s]</t>
-  </si>
-  <si>
-    <t>bug_page</t>
+    <t>myzone_link</t>
+  </si>
+  <si>
+    <t>我的地盘链接</t>
+  </si>
+  <si>
+    <t>main_page</t>
   </si>
   <si>
     <t>xpath</t>
   </si>
   <si>
-    <t>//a[text()=%s]</t>
-  </si>
-  <si>
-    <t>myzone_link</t>
-  </si>
-  <si>
-    <t>我的地盘链接</t>
-  </si>
-  <si>
-    <t>main_page</t>
-  </si>
-  <si>
     <t>//a[@text='我的地盘']</t>
   </si>
   <si>
@@ -109,6 +97,15 @@
   </si>
   <si>
     <t>userNav</t>
+  </si>
+  <si>
+    <t>quit_button</t>
+  </si>
+  <si>
+    <t>退出按钮</t>
+  </si>
+  <si>
+    <t>//a[@href='/zentao/www/index.php?m=user&amp;f=logout']</t>
   </si>
   <si>
     <t>firstpage_link</t>
@@ -754,7 +751,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -762,9 +759,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1086,13 +1080,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20.5357142857143" customWidth="1"/>
     <col min="2" max="3" width="22.3125" customWidth="1"/>
@@ -1181,32 +1175,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D3 D4">
       <formula1>"id,name,class,tag,linktext,plinktext,xpath,css"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1218,19 +1192,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="22.3125" customWidth="1"/>
     <col min="3" max="3" width="26.4821428571429" customWidth="1"/>
     <col min="4" max="4" width="19.6339285714286" customWidth="1"/>
-    <col min="5" max="5" width="22.3214285714286" customWidth="1"/>
+    <col min="5" max="5" width="53.5714285714286" customWidth="1"/>
     <col min="6" max="6" width="10.5625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1256,19 +1230,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -1276,21 +1250,41 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1341,19 +1335,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -1361,19 +1355,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1">
         <v>10</v>

</xml_diff>